<commit_message>
adding 2018 back to the windows data
</commit_message>
<xml_diff>
--- a/Input_Files/20240819_ice_windows.xlsx
+++ b/Input_Files/20240819_ice_windows.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gagers/Documents/Loch Vale &amp; Oleksy/Ice Phenology Project/Ice_Pheno/Input_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BACA8ACA-9C1E-3440-B7F8-742D6E547D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597B4C12-0B3E-E24D-9E46-1051CFE9D216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="17420" xr2:uid="{47EA1361-8AB6-4649-AC66-D6C385E37040}"/>
   </bookViews>
@@ -436,7 +436,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,7 +567,9 @@
       <c r="B8" s="1">
         <v>2018</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="2">
+        <v>43221</v>
+      </c>
       <c r="D8" s="2">
         <v>43228</v>
       </c>

</xml_diff>

<commit_message>
- joined slope data with cumulative Q data - plotted slopes on discharge with pierson ice off dates and visual ice off dates
</commit_message>
<xml_diff>
--- a/Input_Files/20240819_ice_windows.xlsx
+++ b/Input_Files/20240819_ice_windows.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gagers/Documents/Loch Vale &amp; Oleksy/Ice Phenology Project/Ice_Pheno/Input_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597B4C12-0B3E-E24D-9E46-1051CFE9D216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E88788-E637-EA4D-A379-ADAB95808EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="17420" xr2:uid="{47EA1361-8AB6-4649-AC66-D6C385E37040}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
     <t>Loch</t>
   </si>
@@ -55,12 +55,18 @@
   <si>
     <t>Lake</t>
   </si>
+  <si>
+    <t>Pierson_Off_MAX</t>
+  </si>
+  <si>
+    <t>Pierson_Off_AVG</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -70,6 +76,19 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -95,10 +114,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAEDDD4B-84C0-DD43-92F2-1FD2D601C2AA}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -461,6 +485,12 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -559,6 +589,12 @@
       <c r="E7" s="2">
         <v>42885</v>
       </c>
+      <c r="F7" s="5">
+        <v>42880</v>
+      </c>
+      <c r="G7" s="5">
+        <v>42929</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -576,6 +612,12 @@
       <c r="E8" s="2">
         <v>43242</v>
       </c>
+      <c r="F8" s="5">
+        <v>43236</v>
+      </c>
+      <c r="G8" s="5">
+        <v>43241</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -593,6 +635,12 @@
       <c r="E9" s="2">
         <v>43632</v>
       </c>
+      <c r="F9" s="5">
+        <v>43625</v>
+      </c>
+      <c r="G9" s="5">
+        <v>43641</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -610,6 +658,8 @@
       <c r="E10" s="2">
         <v>43973</v>
       </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -626,6 +676,12 @@
       </c>
       <c r="E11" s="2">
         <v>44358</v>
+      </c>
+      <c r="F11" s="5">
+        <v>44353</v>
+      </c>
+      <c r="G11" s="5">
+        <v>44361</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -740,11 +796,71 @@
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="2"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C26" s="4"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C27" s="4"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C28" s="4"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C29" s="4"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C30" s="4"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C31" s="4"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C32" s="4"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C33" s="4"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C34" s="4"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C35" s="4"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C36" s="4"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C37" s="4"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
need pierson dates - highlighted
</commit_message>
<xml_diff>
--- a/Input_Files/20240819_ice_windows.xlsx
+++ b/Input_Files/20240819_ice_windows.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gagers/Documents/Loch Vale &amp; Oleksy/Ice Phenology Project/Ice_Pheno/Input_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E88788-E637-EA4D-A379-ADAB95808EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828348A2-3EC9-5347-9528-63DA6E766FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="17420" xr2:uid="{47EA1361-8AB6-4649-AC66-D6C385E37040}"/>
   </bookViews>
@@ -94,12 +94,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -114,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -123,6 +129,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,13 +469,14 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -485,7 +495,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G1" t="s">
@@ -589,7 +599,7 @@
       <c r="E7" s="2">
         <v>42885</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="7">
         <v>42880</v>
       </c>
       <c r="G7" s="5">
@@ -612,7 +622,7 @@
       <c r="E8" s="2">
         <v>43242</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="7">
         <v>43236</v>
       </c>
       <c r="G8" s="5">
@@ -635,7 +645,7 @@
       <c r="E9" s="2">
         <v>43632</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="7">
         <v>43625</v>
       </c>
       <c r="G9" s="5">
@@ -658,7 +668,7 @@
       <c r="E10" s="2">
         <v>43973</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -677,7 +687,7 @@
       <c r="E11" s="2">
         <v>44358</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="7">
         <v>44353</v>
       </c>
       <c r="G11" s="5">
@@ -722,84 +732,84 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="F19" s="8"/>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="2"/>
+      <c r="F20" s="8"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="F21" s="8"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="F22" s="8"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="F23" s="8"/>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="F24" s="8"/>
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="2"/>
+      <c r="F25" s="8"/>
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.2">

</xml_diff>